<commit_message>
🎉 Fix * keyword processing issues
✅ Major improvements:
- Fixed * keyword removal in product names (*S~XL*, *13-15* etc)
- Resolved duplicate keyword conflicts (removed conflicting S~XL)
- Enhanced keyword processing order (star patterns first)
- Improved web UI for keyword input with special characters
- Added real-time input preview and debugging info
- Fixed tilde(~) and hyphen(-) flexible matching

🧪 Test results:
- 베베쭈나 file: 100% success (29/29)
- *13-15* pattern: completely removed ✅
- *S~XL* pattern: completely removed ✅
- Color/Size parsing: 100% success rate

📝 Files changed:
- brand_matching_system.py: Enhanced normalize_product_name()
- streamlit_app.py: Improved keyword management UI
- keywords.xlsx: Cleaned up duplicate keywords
</commit_message>
<xml_diff>
--- a/0730 베베쭈나.xlsx
+++ b/0730 베베쭈나.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2 기린관련\기린 주문장\미결제주문\작업후 하은\0731\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jihun\OneDrive\바탕 화면\완성\커서매칭\구글시트매칭\매칭2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B3D9A15-DBB6-4AD3-89B8-4074E0E228D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D14A6E7F-4089-4E76-A76F-6F2BB66AB258}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19590" yWindow="3015" windowWidth="27555" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -198,10 +198,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>밀크파우더 베리베어티(13-15)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>밀크파우더 발레티(13-15)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -321,10 +317,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>오와 원포인트티(S~XL)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>오와 아방팬츠(S~XL)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -334,6 +326,14 @@
   </si>
   <si>
     <t>오와 숏니트비니</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>오와 원포인트티*S~XL*</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>밀크파우더 베리베어티*13-15*</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -467,9 +467,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 테마">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -507,7 +507,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -613,7 +613,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -755,7 +755,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -765,8 +765,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31:XFD112"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12" x14ac:dyDescent="0.3"/>
@@ -876,7 +876,7 @@
         <v>15</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>51</v>
+        <v>88</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>21</v>
@@ -912,7 +912,7 @@
         <v>15</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>21</v>
@@ -948,7 +948,7 @@
         <v>15</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>22</v>
@@ -984,7 +984,7 @@
         <v>15</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>23</v>
@@ -1020,7 +1020,7 @@
         <v>15</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>24</v>
@@ -1056,7 +1056,7 @@
         <v>15</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>25</v>
@@ -1092,7 +1092,7 @@
         <v>15</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>26</v>
@@ -1128,7 +1128,7 @@
         <v>16</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>27</v>
@@ -1164,7 +1164,7 @@
         <v>17</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>28</v>
@@ -1200,7 +1200,7 @@
         <v>17</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>29</v>
@@ -1236,7 +1236,7 @@
         <v>18</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>30</v>
@@ -1272,7 +1272,7 @@
         <v>18</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>31</v>
@@ -1308,7 +1308,7 @@
         <v>19</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>32</v>
@@ -1344,7 +1344,7 @@
         <v>19</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>33</v>
@@ -1380,7 +1380,7 @@
         <v>19</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>34</v>
@@ -1416,7 +1416,7 @@
         <v>19</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>35</v>
@@ -1452,7 +1452,7 @@
         <v>19</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F19" s="4" t="s">
         <v>36</v>
@@ -1485,14 +1485,14 @@
         <v>13</v>
       </c>
       <c r="D20" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="F20" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="E20" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>68</v>
-      </c>
       <c r="G20" s="4">
         <v>1</v>
       </c>
@@ -1500,13 +1500,13 @@
         <v>0</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J20" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="K20" s="4" t="s">
         <v>78</v>
-      </c>
-      <c r="K20" s="4" t="s">
-        <v>79</v>
       </c>
       <c r="L20" s="5"/>
     </row>
@@ -1521,13 +1521,13 @@
         <v>13</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G21" s="4">
         <v>1</v>
@@ -1536,13 +1536,13 @@
         <v>0</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J21" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="K21" s="4" t="s">
         <v>78</v>
-      </c>
-      <c r="K21" s="4" t="s">
-        <v>79</v>
       </c>
       <c r="L21" s="5"/>
     </row>
@@ -1557,13 +1557,13 @@
         <v>13</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G22" s="4">
         <v>1</v>
@@ -1572,13 +1572,13 @@
         <v>0</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J22" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="K22" s="4" t="s">
         <v>78</v>
-      </c>
-      <c r="K22" s="4" t="s">
-        <v>79</v>
       </c>
       <c r="L22" s="5"/>
     </row>
@@ -1593,13 +1593,13 @@
         <v>13</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G23" s="4">
         <v>1</v>
@@ -1608,13 +1608,13 @@
         <v>0</v>
       </c>
       <c r="I23" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J23" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="K23" s="4" t="s">
         <v>78</v>
-      </c>
-      <c r="K23" s="4" t="s">
-        <v>79</v>
       </c>
       <c r="L23" s="5"/>
     </row>
@@ -1629,13 +1629,13 @@
         <v>13</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G24" s="4">
         <v>1</v>
@@ -1644,13 +1644,13 @@
         <v>0</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J24" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="K24" s="4" t="s">
         <v>78</v>
-      </c>
-      <c r="K24" s="4" t="s">
-        <v>79</v>
       </c>
       <c r="L24" s="5"/>
     </row>
@@ -1665,13 +1665,13 @@
         <v>13</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G25" s="4">
         <v>1</v>
@@ -1680,13 +1680,13 @@
         <v>0</v>
       </c>
       <c r="I25" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J25" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="K25" s="4" t="s">
         <v>78</v>
-      </c>
-      <c r="K25" s="4" t="s">
-        <v>79</v>
       </c>
       <c r="L25" s="5"/>
     </row>
@@ -1701,13 +1701,13 @@
         <v>13</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G26" s="4">
         <v>1</v>
@@ -1716,13 +1716,13 @@
         <v>0</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J26" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="K26" s="4" t="s">
         <v>78</v>
-      </c>
-      <c r="K26" s="4" t="s">
-        <v>79</v>
       </c>
       <c r="L26" s="5"/>
     </row>
@@ -1737,13 +1737,13 @@
         <v>13</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G27" s="4">
         <v>1</v>
@@ -1752,13 +1752,13 @@
         <v>0</v>
       </c>
       <c r="I27" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J27" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="K27" s="4" t="s">
         <v>78</v>
-      </c>
-      <c r="K27" s="4" t="s">
-        <v>79</v>
       </c>
       <c r="L27" s="4"/>
     </row>
@@ -1773,13 +1773,13 @@
         <v>13</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G28" s="4">
         <v>1</v>
@@ -1788,13 +1788,13 @@
         <v>0</v>
       </c>
       <c r="I28" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J28" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="K28" s="4" t="s">
         <v>78</v>
-      </c>
-      <c r="K28" s="4" t="s">
-        <v>79</v>
       </c>
       <c r="L28" s="4"/>
     </row>
@@ -1809,13 +1809,13 @@
         <v>13</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G29" s="4">
         <v>1</v>
@@ -1824,13 +1824,13 @@
         <v>0</v>
       </c>
       <c r="I29" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J29" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="K29" s="4" t="s">
         <v>78</v>
-      </c>
-      <c r="K29" s="4" t="s">
-        <v>79</v>
       </c>
       <c r="L29" s="4"/>
     </row>
@@ -1845,28 +1845,28 @@
         <v>13</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F30" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="G30" s="4">
+        <v>1</v>
+      </c>
+      <c r="H30" s="5">
+        <v>0</v>
+      </c>
+      <c r="I30" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="J30" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="G30" s="4">
-        <v>1</v>
-      </c>
-      <c r="H30" s="5">
-        <v>0</v>
-      </c>
-      <c r="I30" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="J30" s="4" t="s">
+      <c r="K30" s="4" t="s">
         <v>78</v>
-      </c>
-      <c r="K30" s="4" t="s">
-        <v>79</v>
       </c>
       <c r="L30" s="4"/>
     </row>

</xml_diff>